<commit_message>
bugfix in value conversion for WDI 2015 (and 2016)
</commit_message>
<xml_diff>
--- a/data/Variables.xlsx
+++ b/data/Variables.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/roming/Projects/R-packages/IDA/data-raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/roming/Projects/economic_structure/sf-economic-structure/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-6980" yWindow="-23540" windowWidth="38400" windowHeight="23540" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="860" yWindow="460" windowWidth="24740" windowHeight="15540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="IEA_2014" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3154" uniqueCount="1748">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3155" uniqueCount="1748">
   <si>
     <t>variable</t>
   </si>
@@ -5523,7 +5523,7 @@
     <t>Current account|GDP share</t>
   </si>
   <si>
-    <t>* 100</t>
+    <t>/ 100</t>
   </si>
 </sst>
 </file>
@@ -6011,8 +6011,8 @@
   <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:E1355"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E278" sqref="B278:E278"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1356"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13107,8 +13107,8 @@
       <c r="B1349" s="1" t="s">
         <v>1469</v>
       </c>
-      <c r="C1349" s="1">
-        <v>1</v>
+      <c r="C1349" s="1" t="s">
+        <v>1479</v>
       </c>
       <c r="D1349" s="1" t="s">
         <v>1464</v>
@@ -13237,8 +13237,8 @@
   <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:E1441"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B297" sqref="B297:E297"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E297" sqref="E297"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
include some further variables for historical data
</commit_message>
<xml_diff>
--- a/data/Variables.xlsx
+++ b/data/Variables.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="860" yWindow="460" windowWidth="24740" windowHeight="15540" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="900" yWindow="460" windowWidth="24700" windowHeight="15540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="IEA_2014" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3155" uniqueCount="1748">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3158" uniqueCount="1749">
   <si>
     <t>variable</t>
   </si>
@@ -5524,6 +5524,9 @@
   </si>
   <si>
     <t>/ 100</t>
+  </si>
+  <si>
+    <t>Taxes|Share</t>
   </si>
 </sst>
 </file>
@@ -6012,7 +6015,7 @@
   <dimension ref="A1:E1355"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1356"/>
+      <selection activeCell="B1241" sqref="B1241"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6346,7 +6349,7 @@
         <v>1283</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>1282</v>
       </c>
@@ -6373,7 +6376,7 @@
         <v>1280</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>1279</v>
       </c>
@@ -7015,7 +7018,7 @@
         <v>1154</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A192" s="1" t="s">
         <v>1153</v>
       </c>
@@ -7457,7 +7460,7 @@
         <v>1068</v>
       </c>
     </row>
-    <row r="278" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A278" s="1" t="s">
         <v>1067</v>
       </c>
@@ -7474,7 +7477,7 @@
         <v>1747</v>
       </c>
     </row>
-    <row r="279" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A279" s="1" t="s">
         <v>1066</v>
       </c>
@@ -7946,7 +7949,7 @@
         <v>975</v>
       </c>
     </row>
-    <row r="371" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="371" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A371" s="1" t="s">
         <v>974</v>
       </c>
@@ -7973,7 +7976,7 @@
         <v>972</v>
       </c>
     </row>
-    <row r="374" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="374" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A374" s="1" t="s">
         <v>971</v>
       </c>
@@ -8290,7 +8293,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="435" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="435" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A435" s="1" t="s">
         <v>1482</v>
       </c>
@@ -8323,7 +8326,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="438" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="438" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A438" s="1" t="s">
         <v>1483</v>
       </c>
@@ -8400,7 +8403,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="451" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="451" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A451" s="1" t="s">
         <v>897</v>
       </c>
@@ -8417,7 +8420,7 @@
         <v>1356</v>
       </c>
     </row>
-    <row r="452" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="452" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A452" s="1" t="s">
         <v>896</v>
       </c>
@@ -9024,7 +9027,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="571" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="571" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A571" s="1" t="s">
         <v>8</v>
       </c>
@@ -9057,7 +9060,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="574" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="574" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A574" s="1" t="s">
         <v>10</v>
       </c>
@@ -9164,7 +9167,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="593" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="593" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A593" s="1" t="s">
         <v>760</v>
       </c>
@@ -9197,7 +9200,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="596" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="596" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A596" s="1" t="s">
         <v>757</v>
       </c>
@@ -11014,7 +11017,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="957" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="957" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A957" s="1" t="s">
         <v>396</v>
       </c>
@@ -11926,7 +11929,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="1137" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1137" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1137" s="1" t="s">
         <v>5</v>
       </c>
@@ -12178,7 +12181,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="1185" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1185" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1185" s="1" t="s">
         <v>169</v>
       </c>
@@ -12211,7 +12214,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="1188" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1188" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1188" s="1" t="s">
         <v>166</v>
       </c>
@@ -12373,7 +12376,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="1218" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1218" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1218" s="1" t="s">
         <v>136</v>
       </c>
@@ -12460,82 +12463,94 @@
         <v>122</v>
       </c>
     </row>
-    <row r="1233" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1233" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1233" s="1" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="1234" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1234" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1234" s="1" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="1235" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1235" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1235" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="1236" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1236" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1236" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="1237" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1237" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1237" s="1" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="1238" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1238" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1238" s="1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="1239" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1239" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1239" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="1240" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1240" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1240" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="1241" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1241" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1241" s="1" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="1242" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B1241" s="1" t="s">
+        <v>1748</v>
+      </c>
+      <c r="C1241" s="1" t="s">
+        <v>1464</v>
+      </c>
+      <c r="D1241" s="1">
+        <v>1</v>
+      </c>
+      <c r="E1241" s="1" t="s">
+        <v>1747</v>
+      </c>
+    </row>
+    <row r="1242" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1242" s="1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="1243" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1243" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1243" s="1" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="1244" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1244" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1244" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="1245" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1245" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1245" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="1246" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1246" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1246" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="1247" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1247" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1247" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="1248" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1248" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1248" s="1" t="s">
         <v>106</v>
       </c>
@@ -12895,7 +12910,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="1320" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1320" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1320" s="1" t="s">
         <v>6</v>
       </c>
@@ -13032,7 +13047,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="1345" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1345" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1345" s="1" t="s">
         <v>911</v>
       </c>
@@ -13049,7 +13064,7 @@
         <v>1361</v>
       </c>
     </row>
-    <row r="1346" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1346" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1346" s="1" t="s">
         <v>612</v>
       </c>
@@ -13066,7 +13081,7 @@
         <v>1356</v>
       </c>
     </row>
-    <row r="1347" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1347" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1347" s="1" t="s">
         <v>912</v>
       </c>
@@ -13083,7 +13098,7 @@
         <v>1361</v>
       </c>
     </row>
-    <row r="1348" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1348" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1348" s="1" t="s">
         <v>625</v>
       </c>
@@ -13100,7 +13115,7 @@
         <v>1356</v>
       </c>
     </row>
-    <row r="1349" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1349" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1349" s="1" t="s">
         <v>988</v>
       </c>
@@ -13117,7 +13132,7 @@
         <v>1361</v>
       </c>
     </row>
-    <row r="1350" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1350" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1350" s="1" t="s">
         <v>987</v>
       </c>
@@ -13134,7 +13149,7 @@
         <v>1361</v>
       </c>
     </row>
-    <row r="1351" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1351" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1351" s="1" t="s">
         <v>1203</v>
       </c>
@@ -13151,7 +13166,7 @@
         <v>1361</v>
       </c>
     </row>
-    <row r="1352" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1352" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1352" s="1" t="s">
         <v>892</v>
       </c>
@@ -13168,7 +13183,7 @@
         <v>1356</v>
       </c>
     </row>
-    <row r="1353" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1353" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1353" s="1" t="s">
         <v>634</v>
       </c>
@@ -13185,7 +13200,7 @@
         <v>1356</v>
       </c>
     </row>
-    <row r="1354" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1354" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1354" s="1" t="s">
         <v>631</v>
       </c>
@@ -13202,7 +13217,7 @@
         <v>1356</v>
       </c>
     </row>
-    <row r="1355" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1355" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1355" s="1" t="s">
         <v>233</v>
       </c>
@@ -13221,10 +13236,10 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:E1355">
-    <filterColumn colId="1">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Taxes on goods and services (% value added of industry and services)"/>
+      </filters>
     </filterColumn>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
include urban population share in data
</commit_message>
<xml_diff>
--- a/data/Variables.xlsx
+++ b/data/Variables.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28109"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28209"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="24600" windowHeight="15540" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="1260" yWindow="-20540" windowWidth="24600" windowHeight="15540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="IEA_2014" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3167" uniqueCount="1752">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3170" uniqueCount="1754">
   <si>
     <t>variable</t>
   </si>
@@ -5536,6 +5536,12 @@
   </si>
   <si>
     <t>Value Added|Services|GDP share</t>
+  </si>
+  <si>
+    <t>Population|Urban|Share</t>
+  </si>
+  <si>
+    <t>/100</t>
   </si>
 </sst>
 </file>
@@ -6022,8 +6028,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1355"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1165" workbookViewId="0">
-      <selection activeCell="B1178" sqref="B1178"/>
+    <sheetView tabSelected="1" topLeftCell="A1302" workbookViewId="0">
+      <selection activeCell="F1321" sqref="F1321"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12974,6 +12980,18 @@
     <row r="1321" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1321" s="1" t="s">
         <v>34</v>
+      </c>
+      <c r="B1321" s="1" t="s">
+        <v>1752</v>
+      </c>
+      <c r="C1321" s="1" t="s">
+        <v>1464</v>
+      </c>
+      <c r="D1321" s="1">
+        <v>1</v>
+      </c>
+      <c r="E1321" s="1" t="s">
+        <v>1753</v>
       </c>
     </row>
     <row r="1322" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>